<commit_message>
Updated health insurance, traditional finance models
Total updates:

UNH
WU
MOH
</commit_message>
<xml_diff>
--- a/Health Insurance/UNH_MODEL.xlsx
+++ b/Health Insurance/UNH_MODEL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Health Insurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D090685-A0D8-4772-83F0-4F03EA2C3169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA33D6A-DE0B-4EA2-BCA1-7E25506A7BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t>Price</t>
   </si>
@@ -445,9 +445,6 @@
     <t xml:space="preserve">Rest 2030+ </t>
   </si>
   <si>
-    <t>Net EPS 14.65, 16</t>
-  </si>
-  <si>
     <t>FY 445.5 to 448 bill</t>
   </si>
   <si>
@@ -458,6 +455,12 @@
   </si>
   <si>
     <t>Q42017</t>
+  </si>
+  <si>
+    <t>MCR</t>
+  </si>
+  <si>
+    <t>Raise to 14.90 NET EPS, adjusted 16.25</t>
   </si>
 </sst>
 </file>
@@ -469,13 +472,19 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -647,60 +656,60 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1040,7 +1049,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1071,10 +1080,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>247.8</v>
+        <v>307.26</v>
       </c>
       <c r="C4" s="2">
-        <v>45876</v>
+        <v>45980</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1082,10 +1091,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>913</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>905.8</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1094,7 +1103,7 @@
       </c>
       <c r="B6" s="1">
         <f xml:space="preserve"> B4 * B5</f>
-        <v>226241.40000000002</v>
+        <v>278316.10799999995</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1102,7 +1111,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="1">
-        <v>32</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1110,13 +1119,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="1">
-        <v>4.32</v>
+        <v>33.799999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1125,13 +1134,13 @@
       </c>
       <c r="B9" s="1">
         <f>B6 - B7 + B8</f>
-        <v>226288.40000000002</v>
+        <v>278365.50799999997</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="1">
-        <v>5.27</v>
+        <v>105.72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1139,7 +1148,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="1">
-        <v>0.54</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1147,7 +1156,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="1">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1155,7 +1164,7 @@
         <v>46</v>
       </c>
       <c r="B13" s="1">
-        <v>8.74</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1163,7 +1172,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="1">
-        <v>0.69</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1171,7 +1180,7 @@
         <v>48</v>
       </c>
       <c r="B15" s="1">
-        <v>11</v>
+        <v>16.78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1179,7 +1188,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="1">
-        <v>14</v>
+        <v>10.76</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -1200,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
-  <dimension ref="A1:AR96"/>
+  <dimension ref="A1:AR97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="K17" workbookViewId="0">
+      <selection activeCell="AI61" sqref="AI61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1234,10 +1243,10 @@
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>115</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>116</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>71</v>
@@ -1261,7 +1270,7 @@
         <v>61</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>60</v>
@@ -1339,8 +1348,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1431,7 +1440,7 @@
       <c r="AH4" s="1">
         <v>19066</v>
       </c>
-      <c r="AI4" s="36">
+      <c r="AI4" s="1">
         <v>18950</v>
       </c>
     </row>
@@ -2165,6 +2174,9 @@
       <c r="AI15" s="1">
         <v>8.4</v>
       </c>
+      <c r="AJ15" s="1">
+        <v>8.4</v>
+      </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
@@ -2264,6 +2276,9 @@
         <v>21.6</v>
       </c>
       <c r="AI16" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="AJ16" s="1">
         <v>21.5</v>
       </c>
     </row>
@@ -2279,67 +2294,67 @@
       <c r="E17" s="27">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="34">
         <v>4.5</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="34">
         <v>4.8</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="34">
         <v>4.9000000000000004</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="34">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J17" s="38">
+      <c r="J17" s="34">
         <v>5.2</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="34">
         <v>5.2</v>
       </c>
-      <c r="L17" s="38">
+      <c r="L17" s="34">
         <v>5.2</v>
       </c>
-      <c r="M17" s="38">
+      <c r="M17" s="34">
         <v>5.3</v>
       </c>
-      <c r="N17" s="38">
+      <c r="N17" s="34">
         <v>5.6</v>
       </c>
-      <c r="O17" s="38">
+      <c r="O17" s="34">
         <v>5.6</v>
       </c>
-      <c r="P17" s="38">
+      <c r="P17" s="34">
         <v>5.7</v>
       </c>
-      <c r="Q17" s="38">
+      <c r="Q17" s="34">
         <v>5.7</v>
       </c>
-      <c r="R17" s="38">
+      <c r="R17" s="34">
         <v>6.3</v>
       </c>
-      <c r="S17" s="38">
+      <c r="S17" s="34">
         <v>6.4</v>
       </c>
-      <c r="T17" s="38">
+      <c r="T17" s="34">
         <v>6.5</v>
       </c>
-      <c r="U17" s="38">
+      <c r="U17" s="34">
         <v>6.5</v>
       </c>
-      <c r="V17" s="38">
+      <c r="V17" s="34">
         <v>6.8</v>
       </c>
-      <c r="W17" s="38">
+      <c r="W17" s="34">
         <v>6.9</v>
       </c>
-      <c r="X17" s="38">
+      <c r="X17" s="34">
         <v>7</v>
       </c>
-      <c r="Y17" s="38">
+      <c r="Y17" s="34">
         <v>7.1</v>
       </c>
-      <c r="Z17" s="38">
+      <c r="Z17" s="34">
         <v>7.5</v>
       </c>
       <c r="AA17" s="1">
@@ -2368,6 +2383,9 @@
       </c>
       <c r="AI17" s="1">
         <v>8.3000000000000007</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>8.4</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.2">
@@ -2382,67 +2400,67 @@
       <c r="E18" s="27">
         <v>6.7</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="34">
         <v>6.7</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="34">
         <v>6.7</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="34">
         <v>6.6</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="34">
         <v>6.5</v>
       </c>
-      <c r="J18" s="38">
+      <c r="J18" s="34">
         <v>6.4</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="34">
         <v>6.4</v>
       </c>
-      <c r="L18" s="38">
+      <c r="L18" s="34">
         <v>6</v>
       </c>
-      <c r="M18" s="38">
+      <c r="M18" s="34">
         <v>5.9</v>
       </c>
-      <c r="N18" s="38">
+      <c r="N18" s="34">
         <v>5.9</v>
       </c>
-      <c r="O18" s="38">
+      <c r="O18" s="34">
         <v>6.2</v>
       </c>
-      <c r="P18" s="38">
+      <c r="P18" s="34">
         <v>6.4</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="34">
         <v>6.6</v>
       </c>
-      <c r="R18" s="38">
+      <c r="R18" s="34">
         <v>7</v>
       </c>
-      <c r="S18" s="38">
+      <c r="S18" s="34">
         <v>7.1</v>
       </c>
-      <c r="T18" s="38">
+      <c r="T18" s="34">
         <v>7.5</v>
       </c>
-      <c r="U18" s="38">
+      <c r="U18" s="34">
         <v>7.6</v>
       </c>
-      <c r="V18" s="38">
+      <c r="V18" s="34">
         <v>7.8</v>
       </c>
-      <c r="W18" s="38">
+      <c r="W18" s="34">
         <v>8</v>
       </c>
-      <c r="X18" s="38">
+      <c r="X18" s="34">
         <v>8</v>
       </c>
-      <c r="Y18" s="38">
+      <c r="Y18" s="34">
         <v>8.1999999999999993</v>
       </c>
-      <c r="Z18" s="38">
+      <c r="Z18" s="34">
         <v>8.3000000000000007</v>
       </c>
       <c r="AA18" s="1">
@@ -2470,6 +2488,9 @@
         <v>7.5</v>
       </c>
       <c r="AI18" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="AJ18" s="1">
         <v>7.5</v>
       </c>
     </row>
@@ -2485,67 +2506,67 @@
       <c r="E19" s="27">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="34">
         <v>4.5</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="34">
         <v>4.5</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="34">
         <v>4.5</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="34">
         <v>4.5</v>
       </c>
-      <c r="J19" s="38">
+      <c r="J19" s="34">
         <v>4.5</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="34">
         <v>4.5</v>
       </c>
-      <c r="L19" s="38">
+      <c r="L19" s="34">
         <v>4.5</v>
       </c>
-      <c r="M19" s="38">
+      <c r="M19" s="34">
         <v>4.5</v>
       </c>
-      <c r="N19" s="38">
+      <c r="N19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="O19" s="38">
+      <c r="O19" s="34">
         <v>4.5</v>
       </c>
-      <c r="P19" s="38">
+      <c r="P19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="34">
         <v>4.5</v>
       </c>
-      <c r="R19" s="38">
+      <c r="R19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="S19" s="38">
+      <c r="S19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="T19" s="38">
+      <c r="T19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="U19" s="38">
+      <c r="U19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="V19" s="38">
+      <c r="V19" s="34">
         <v>4.3</v>
       </c>
-      <c r="W19" s="38">
+      <c r="W19" s="34">
         <v>4.3</v>
       </c>
-      <c r="X19" s="38">
+      <c r="X19" s="34">
         <v>4.3</v>
       </c>
-      <c r="Y19" s="38">
+      <c r="Y19" s="34">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Z19" s="38">
+      <c r="Z19" s="34">
         <v>4.3</v>
       </c>
       <c r="AA19" s="1">
@@ -2573,6 +2594,9 @@
         <v>4.3</v>
       </c>
       <c r="AI19" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="AJ19" s="1">
         <v>4.3</v>
       </c>
     </row>
@@ -2710,6 +2734,9 @@
         <f>SUM(AI17:AI19)</f>
         <v>20.100000000000001</v>
       </c>
+      <c r="AJ20" s="8">
+        <v>20.2</v>
+      </c>
     </row>
     <row r="21" spans="1:38" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
@@ -2805,7 +2832,7 @@
         <v>50.6</v>
       </c>
       <c r="AG21" s="8">
-        <f t="shared" ref="H21:AH21" si="3">SUM(AG15:AG19)</f>
+        <f t="shared" ref="AG21:AH21" si="3">SUM(AG15:AG19)</f>
         <v>49.199999999999996</v>
       </c>
       <c r="AH21" s="8">
@@ -2814,6 +2841,9 @@
       </c>
       <c r="AI21" s="8">
         <f>SUM(AI15:AI19)</f>
+        <v>50</v>
+      </c>
+      <c r="AJ21" s="8">
         <v>50</v>
       </c>
     </row>
@@ -2949,6 +2979,9 @@
       <c r="AI23" s="1">
         <v>87905</v>
       </c>
+      <c r="AJ23" s="1">
+        <v>88979</v>
+      </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
@@ -3052,6 +3085,9 @@
       <c r="AI24" s="1">
         <v>13564</v>
       </c>
+      <c r="AJ24" s="1">
+        <v>13296</v>
+      </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
@@ -3155,6 +3191,9 @@
       <c r="AI25" s="1">
         <v>9039</v>
       </c>
+      <c r="AJ25" s="1">
+        <v>9754</v>
+      </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
@@ -3257,6 +3296,9 @@
       </c>
       <c r="AI26" s="1">
         <v>1108</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>1132</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.2">
@@ -3423,7 +3465,7 @@
       </c>
       <c r="AJ28" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>113161</v>
       </c>
       <c r="AK28" s="3">
         <f t="shared" si="5"/>
@@ -3536,6 +3578,9 @@
       <c r="AI29" s="1">
         <v>78585</v>
       </c>
+      <c r="AJ29" s="1">
+        <v>79958</v>
+      </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
@@ -3639,6 +3684,9 @@
       <c r="AI30" s="17">
         <v>13778</v>
       </c>
+      <c r="AJ30" s="1">
+        <v>15223</v>
+      </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
@@ -3742,6 +3790,9 @@
       <c r="AI31" s="28">
         <v>13019</v>
       </c>
+      <c r="AJ31" s="1">
+        <v>12566</v>
+      </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
@@ -3845,6 +3896,9 @@
       <c r="AI32" s="28">
         <v>1084</v>
       </c>
+      <c r="AJ32" s="1">
+        <v>1099</v>
+      </c>
     </row>
     <row r="33" spans="1:40" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
@@ -3981,7 +4035,7 @@
       </c>
       <c r="AJ33" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4315</v>
       </c>
       <c r="AK33" s="4">
         <f t="shared" si="6"/>
@@ -4096,6 +4150,9 @@
       <c r="AI34" s="1">
         <v>4082</v>
       </c>
+      <c r="AJ34" s="1">
+        <v>3229</v>
+      </c>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
@@ -4197,6 +4254,9 @@
       <c r="AI35" s="1">
         <v>510</v>
       </c>
+      <c r="AJ35" s="1">
+        <v>686</v>
+      </c>
     </row>
     <row r="36" spans="1:40" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
@@ -4215,7 +4275,7 @@
         <v>2924</v>
       </c>
       <c r="G36" s="5">
-        <f t="shared" ref="F36:Q36" si="8">G34-G35</f>
+        <f t="shared" ref="G36:Q36" si="8">G34-G35</f>
         <v>3010</v>
       </c>
       <c r="H36" s="5">
@@ -4332,7 +4392,7 @@
       </c>
       <c r="AJ36" s="5">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2543</v>
       </c>
       <c r="AK36" s="5">
         <f t="shared" si="11"/>
@@ -4448,6 +4508,9 @@
       <c r="AI37" s="1">
         <v>3.74</v>
       </c>
+      <c r="AJ37" s="1">
+        <v>2.59</v>
+      </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
@@ -4549,6 +4612,9 @@
       <c r="AI38" s="1">
         <v>4.08</v>
       </c>
+      <c r="AJ38" s="1">
+        <v>2.92</v>
+      </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
@@ -4575,110 +4641,113 @@
         <v>0.11779338321118993</v>
       </c>
       <c r="J40" s="6">
-        <f>(J28/F28) - 1</f>
+        <f t="shared" ref="J40:AJ40" si="13">(J28/F28) - 1</f>
         <v>9.2773791403928385E-2</v>
       </c>
       <c r="K40" s="6">
-        <f>(K28/G28) - 1</f>
+        <f t="shared" si="13"/>
         <v>8.0394394323003882E-2</v>
       </c>
       <c r="L40" s="6">
-        <f>(L28/H28) - 1</f>
+        <f t="shared" si="13"/>
         <v>6.7101633778909431E-2</v>
       </c>
       <c r="M40" s="6">
-        <f>(M28/I28) - 1</f>
+        <f t="shared" si="13"/>
         <v>4.2521868634130433E-2</v>
       </c>
       <c r="N40" s="6">
-        <f>(N28/J28) - 1</f>
+        <f t="shared" si="13"/>
         <v>6.8199907143330796E-2</v>
       </c>
       <c r="O40" s="6">
-        <f>(O28/K28) - 1</f>
+        <f t="shared" si="13"/>
         <v>2.5464147206865295E-2</v>
       </c>
       <c r="P40" s="6">
-        <f>(P28/L28) - 1</f>
+        <f t="shared" si="13"/>
         <v>7.8938211462941776E-2</v>
       </c>
       <c r="Q40" s="6">
-        <f>(Q28/M28) - 1</f>
+        <f t="shared" si="13"/>
         <v>7.497413835569211E-2</v>
       </c>
       <c r="R40" s="6">
-        <f>(R28/N28) - 1</f>
+        <f t="shared" si="13"/>
         <v>8.9644681082255762E-2</v>
       </c>
       <c r="S40" s="6">
-        <f>(S28/O28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.14778396472367961</v>
       </c>
       <c r="T40" s="6">
-        <f>(T28/P28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.11091146433233501</v>
       </c>
       <c r="U40" s="6">
-        <f>(U28/Q28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.1264148349550156</v>
       </c>
       <c r="V40" s="6">
-        <f>(V28/R28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.1417887059091687</v>
       </c>
       <c r="W40" s="6">
-        <f>(W28/S28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.12634427447736285</v>
       </c>
       <c r="X40" s="6">
-        <f>(X28/T28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.11829354272364068</v>
       </c>
       <c r="Y40" s="6">
-        <f>(Y28/U28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.12264214908533688</v>
       </c>
       <c r="Z40" s="6">
-        <f>(Z28/V28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.14700121024591706</v>
       </c>
       <c r="AA40" s="6">
-        <f>(AA28/W28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.15648807449086299</v>
       </c>
       <c r="AB40" s="6">
-        <f>(AB28/X28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.14175340569139872</v>
       </c>
       <c r="AC40" s="6">
-        <f>(AC28/Y28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.14060178530445611</v>
       </c>
       <c r="AD40" s="6">
-        <f>(AD28/Z28) - 1</f>
+        <f t="shared" si="13"/>
         <v>8.5553295406337382E-2</v>
       </c>
       <c r="AE40" s="6">
-        <f>(AE28/AA28) - 1</f>
+        <f t="shared" si="13"/>
         <v>6.4066822384637678E-2</v>
       </c>
       <c r="AF40" s="6">
-        <f>(AF28/AB28) - 1</f>
+        <f t="shared" si="13"/>
         <v>9.158627559251209E-2</v>
       </c>
       <c r="AG40" s="6">
-        <f>(AG28/AC28) - 1</f>
+        <f t="shared" si="13"/>
         <v>6.7565420907155893E-2</v>
       </c>
       <c r="AH40" s="6">
-        <f>(AH28/AD28) - 1</f>
+        <f t="shared" si="13"/>
         <v>9.8070062928373947E-2</v>
       </c>
       <c r="AI40" s="6">
-        <f>(AI28/AE28) - 1</f>
+        <f t="shared" si="13"/>
         <v>0.12908805826715897</v>
       </c>
-      <c r="AJ40" s="6"/>
+      <c r="AJ40" s="6">
+        <f t="shared" si="13"/>
+        <v>0.12240626859750048</v>
+      </c>
       <c r="AK40" s="6"/>
       <c r="AL40" s="6"/>
       <c r="AM40" s="6"/>
@@ -4692,130 +4761,133 @@
         <v>41</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" ref="E41:F41" si="13" xml:space="preserve"> (E28/D28) - 1</f>
+        <f t="shared" ref="E41:F41" si="14" xml:space="preserve"> (E28/D28) - 1</f>
         <v>3.8531854854735537E-2</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.6007347735405055E-2</v>
       </c>
       <c r="G41" s="6">
-        <f xml:space="preserve"> (G28/F28) - 1</f>
+        <f t="shared" ref="G41:AJ41" si="15" xml:space="preserve"> (G28/F28) - 1</f>
         <v>1.6271653257954544E-2</v>
       </c>
       <c r="H41" s="6">
-        <f xml:space="preserve"> (H28/G28) - 1</f>
+        <f t="shared" si="15"/>
         <v>8.3799878757622182E-3</v>
       </c>
       <c r="I41" s="6">
-        <f xml:space="preserve"> (I28/H28) - 1</f>
+        <f t="shared" si="15"/>
         <v>3.2905438857061986E-2</v>
       </c>
       <c r="J41" s="6">
-        <f xml:space="preserve"> (J28/I28) - 1</f>
+        <f t="shared" si="15"/>
         <v>3.2370714004485102E-2</v>
       </c>
       <c r="K41" s="6">
-        <f xml:space="preserve"> (K28/J28) - 1</f>
+        <f t="shared" si="15"/>
         <v>4.7589042913045443E-3</v>
       </c>
       <c r="L41" s="6">
-        <f xml:space="preserve"> (L28/K28) - 1</f>
+        <f t="shared" si="15"/>
         <v>-4.0267348791154234E-3</v>
       </c>
       <c r="M41" s="6">
-        <f xml:space="preserve"> (M28/L28) - 1</f>
+        <f t="shared" si="15"/>
         <v>9.113353548408476E-3</v>
       </c>
       <c r="N41" s="6">
-        <f xml:space="preserve"> (N28/M28) - 1</f>
+        <f t="shared" si="15"/>
         <v>5.7798722516871681E-2</v>
       </c>
       <c r="O41" s="6">
-        <f xml:space="preserve"> (O28/N28) - 1</f>
+        <f t="shared" si="15"/>
         <v>-3.5438754443426812E-2</v>
       </c>
       <c r="P41" s="6">
-        <f xml:space="preserve"> (P28/O28) - 1</f>
+        <f t="shared" si="15"/>
         <v>4.7909491776368718E-2</v>
       </c>
       <c r="Q41" s="6">
-        <f xml:space="preserve"> (Q28/P28) - 1</f>
+        <f t="shared" si="15"/>
         <v>5.4058204714735325E-3</v>
       </c>
       <c r="R41" s="6">
-        <f xml:space="preserve"> (R28/Q28) - 1</f>
+        <f t="shared" si="15"/>
         <v>7.2234866421250432E-2</v>
       </c>
       <c r="S41" s="6">
-        <f xml:space="preserve"> (S28/R28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.6026554219613631E-2</v>
       </c>
       <c r="T41" s="6">
-        <f xml:space="preserve"> (T28/S28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.4245453653201734E-2</v>
       </c>
       <c r="U41" s="6">
-        <f xml:space="preserve"> (U28/T28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.9436802742718085E-2</v>
       </c>
       <c r="V41" s="6">
-        <f xml:space="preserve"> (V28/U28) - 1</f>
+        <f t="shared" si="15"/>
         <v>8.6869262167256656E-2</v>
       </c>
       <c r="W41" s="6">
-        <f xml:space="preserve"> (W28/V28) - 1</f>
+        <f t="shared" si="15"/>
         <v>2.2832474516214507E-3</v>
       </c>
       <c r="X41" s="6">
-        <f xml:space="preserve"> (X28/W28) - 1</f>
+        <f t="shared" si="15"/>
         <v>6.9959667380370405E-3</v>
       </c>
       <c r="Y41" s="6">
-        <f xml:space="preserve"> (Y28/X28) - 1</f>
+        <f t="shared" si="15"/>
         <v>2.3400993893242905E-2</v>
       </c>
       <c r="Z41" s="6">
-        <f xml:space="preserve"> (Z28/Y28) - 1</f>
+        <f t="shared" si="15"/>
         <v>0.11045212412576855</v>
       </c>
       <c r="AA41" s="6">
-        <f xml:space="preserve"> (AA28/Z28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.0573147251743187E-2</v>
       </c>
       <c r="AB41" s="6">
-        <f xml:space="preserve"> (AB28/AA28) - 1</f>
+        <f t="shared" si="15"/>
         <v>-5.8340419577408431E-3</v>
       </c>
       <c r="AC41" s="6">
-        <f xml:space="preserve"> (AC28/AB28) - 1</f>
+        <f t="shared" si="15"/>
         <v>2.236874871428407E-2</v>
       </c>
       <c r="AD41" s="6">
-        <f xml:space="preserve"> (AD28/AC28) - 1</f>
+        <f t="shared" si="15"/>
         <v>5.6858737437385454E-2</v>
       </c>
       <c r="AE41" s="6">
-        <f xml:space="preserve"> (AE28/AD28) - 1</f>
+        <f t="shared" si="15"/>
         <v>-9.4292356407070788E-3</v>
       </c>
       <c r="AF41" s="6">
-        <f xml:space="preserve"> (AF28/AE28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.9877598502857641E-2</v>
       </c>
       <c r="AG41" s="6">
-        <f xml:space="preserve"> (AG28/AF28) - 1</f>
+        <f t="shared" si="15"/>
         <v>-1.289426701051033E-4</v>
       </c>
       <c r="AH41" s="6">
-        <f xml:space="preserve"> (AH28/AG28) - 1</f>
+        <f t="shared" si="15"/>
         <v>8.7057446407491579E-2</v>
       </c>
       <c r="AI41" s="6">
-        <f xml:space="preserve"> (AI28/AH28) - 1</f>
+        <f t="shared" si="15"/>
         <v>1.8552147687141307E-2</v>
       </c>
-      <c r="AJ41" s="6"/>
+      <c r="AJ41" s="6">
+        <f t="shared" si="15"/>
+        <v>1.3842101490825653E-2</v>
+      </c>
       <c r="AK41" s="6"/>
       <c r="AL41" s="6"/>
       <c r="AM41" s="6"/>
@@ -4834,1017 +4906,1027 @@
       <c r="AG42" s="7"/>
       <c r="AH42" s="6"/>
     </row>
-    <row r="43" spans="1:40" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="37" t="s">
+    <row r="43" spans="1:40" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="37">
+      <c r="D43" s="33">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="E43" s="37">
+      <c r="E43" s="33">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F43" s="37">
+      <c r="F43" s="33">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="G43" s="37">
+      <c r="G43" s="33">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H43" s="37">
+      <c r="H43" s="33">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I43" s="37">
+      <c r="I43" s="33">
         <v>3.9E-2</v>
       </c>
-      <c r="J43" s="37">
+      <c r="J43" s="33">
         <v>0.06</v>
       </c>
-      <c r="K43" s="37">
+      <c r="K43" s="33">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="L43" s="37">
+      <c r="L43" s="33">
         <v>5.5E-2</v>
       </c>
-      <c r="M43" s="37">
+      <c r="M43" s="33">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="N43" s="37">
+      <c r="N43" s="33">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="O43" s="37">
+      <c r="O43" s="33">
         <v>0.14299999999999999</v>
       </c>
-      <c r="P43" s="37">
+      <c r="P43" s="33">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="Q43" s="37">
+      <c r="Q43" s="33">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R43" s="37">
+      <c r="R43" s="33">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="S43" s="37">
+      <c r="S43" s="33">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="T43" s="37">
+      <c r="T43" s="33">
         <v>4.7E-2</v>
       </c>
-      <c r="U43" s="37">
+      <c r="U43" s="33">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="V43" s="37">
+      <c r="V43" s="33">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="W43" s="37">
+      <c r="W43" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="X43" s="37">
+      <c r="X43" s="33">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="Y43" s="37">
+      <c r="Y43" s="33">
         <v>4.7E-2</v>
       </c>
-      <c r="Z43" s="37">
+      <c r="Z43" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="AA43" s="37">
+      <c r="AA43" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="AB43" s="37">
+      <c r="AB43" s="33">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="AC43" s="37">
+      <c r="AC43" s="33">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="AD43" s="37">
+      <c r="AD43" s="33">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="AE43" s="37">
+      <c r="AE43" s="33">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="AF43" s="37">
+      <c r="AF43" s="33">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="AG43" s="37">
+      <c r="AG43" s="33">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="AH43" s="37">
+      <c r="AH43" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="AI43" s="37">
+      <c r="AI43" s="33">
         <v>2.4E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:40" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="37" t="s">
+      <c r="AJ43" s="33">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:40" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="D44" s="37">
+      <c r="D44" s="33">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E44" s="37">
+      <c r="E44" s="33">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="F44" s="37">
+      <c r="F44" s="33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G44" s="37">
+      <c r="G44" s="33">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="H44" s="37">
+      <c r="H44" s="33">
         <v>0.08</v>
       </c>
-      <c r="I44" s="37">
+      <c r="I44" s="33">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="J44" s="37">
+      <c r="J44" s="33">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="K44" s="37">
+      <c r="K44" s="33">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="L44" s="37">
+      <c r="L44" s="33">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="M44" s="37">
+      <c r="M44" s="33">
         <v>0.10100000000000001</v>
       </c>
-      <c r="N44" s="37">
+      <c r="N44" s="33">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="O44" s="37">
+      <c r="O44" s="33">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="P44" s="37">
+      <c r="P44" s="33">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="Q44" s="37">
+      <c r="Q44" s="33">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="R44" s="37">
+      <c r="R44" s="33">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S44" s="37">
+      <c r="S44" s="33">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="T44" s="37">
+      <c r="T44" s="33">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="U44" s="37">
+      <c r="U44" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="V44" s="37">
+      <c r="V44" s="33">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="W44" s="37">
+      <c r="W44" s="33">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="X44" s="37">
+      <c r="X44" s="33">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="Y44" s="37">
+      <c r="Y44" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="Z44" s="37">
+      <c r="Z44" s="33">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="AA44" s="37">
+      <c r="AA44" s="33">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="AB44" s="37">
+      <c r="AB44" s="33">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="AC44" s="37">
+      <c r="AC44" s="33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AD44" s="37">
+      <c r="AD44" s="33">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="AE44" s="37">
+      <c r="AE44" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="AF44" s="37">
+      <c r="AF44" s="33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AG44" s="37">
+      <c r="AG44" s="33">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="AH44" s="37">
+      <c r="AH44" s="33">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="AI44" s="37">
+      <c r="AI44" s="33">
         <v>4.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:40" s="37" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="37" t="s">
+      <c r="AJ44" s="33">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:40" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="37">
+      <c r="D45" s="33">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E45" s="37">
+      <c r="E45" s="33">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="F45" s="37">
+      <c r="F45" s="33">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G45" s="37">
+      <c r="G45" s="33">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="H45" s="37">
+      <c r="H45" s="33">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I45" s="37">
+      <c r="I45" s="33">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J45" s="37">
+      <c r="J45" s="33">
         <v>0.08</v>
       </c>
-      <c r="K45" s="37">
+      <c r="K45" s="33">
         <v>7.8E-2</v>
       </c>
-      <c r="L45" s="37">
+      <c r="L45" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="M45" s="37">
+      <c r="M45" s="33">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="N45" s="37">
+      <c r="N45" s="33">
         <v>7.8E-2</v>
       </c>
-      <c r="O45" s="37">
+      <c r="O45" s="33">
         <v>0.14899999999999999</v>
       </c>
-      <c r="P45" s="37">
+      <c r="P45" s="33">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="Q45" s="37">
+      <c r="Q45" s="33">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="R45" s="37">
+      <c r="R45" s="33">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="S45" s="37">
+      <c r="S45" s="33">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="T45" s="37">
+      <c r="T45" s="33">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="U45" s="37">
+      <c r="U45" s="33">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="V45" s="37">
+      <c r="V45" s="33">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="W45" s="37">
+      <c r="W45" s="33">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="X45" s="37">
+      <c r="X45" s="33">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="Y45" s="37">
+      <c r="Y45" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="Z45" s="37">
+      <c r="Z45" s="33">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="AA45" s="37">
+      <c r="AA45" s="33">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="AB45" s="37">
+      <c r="AB45" s="33">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="AC45" s="37">
+      <c r="AC45" s="33">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="AD45" s="37">
+      <c r="AD45" s="33">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="AE45" s="37">
+      <c r="AE45" s="33">
         <v>0.08</v>
       </c>
-      <c r="AF45" s="37">
+      <c r="AF45" s="33">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="AG45" s="37">
+      <c r="AG45" s="33">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="AH45" s="37">
+      <c r="AH45" s="33">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="AI45" s="37">
+      <c r="AI45" s="33">
         <v>4.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:40" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="30" t="s">
+      <c r="AJ45" s="33">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:40" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ46" s="33">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:40" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30">
+      <c r="C48" s="30"/>
+      <c r="D48" s="30">
         <v>7546</v>
       </c>
-      <c r="E47" s="30">
+      <c r="E48" s="30">
         <v>-2577</v>
       </c>
-      <c r="F47" s="30">
+      <c r="F48" s="30">
         <v>8369</v>
       </c>
-      <c r="G47" s="30">
+      <c r="G48" s="30">
         <v>4007</v>
       </c>
-      <c r="H47" s="30">
+      <c r="H48" s="30">
         <v>941</v>
       </c>
-      <c r="I47" s="30">
+      <c r="I48" s="30">
         <v>2396</v>
       </c>
-      <c r="J47" s="30">
+      <c r="J48" s="30">
         <v>3234</v>
       </c>
-      <c r="K47" s="30">
+      <c r="K48" s="30">
         <v>5874</v>
       </c>
-      <c r="L47" s="30">
+      <c r="L48" s="30">
         <v>3150</v>
       </c>
-      <c r="M47" s="30">
+      <c r="M48" s="30">
         <v>6205</v>
       </c>
-      <c r="N47" s="30">
+      <c r="N48" s="30">
         <v>2943</v>
       </c>
-      <c r="O47" s="30">
+      <c r="O48" s="30">
         <v>10003</v>
       </c>
-      <c r="P47" s="30">
+      <c r="P48" s="30">
         <v>3127</v>
       </c>
-      <c r="Q47" s="30">
+      <c r="Q48" s="30">
         <v>6101</v>
       </c>
-      <c r="R47" s="30">
+      <c r="R48" s="30">
         <v>6005</v>
       </c>
-      <c r="S47" s="30">
+      <c r="S48" s="30">
         <v>5540</v>
       </c>
-      <c r="T47" s="30">
+      <c r="T48" s="30">
         <v>7580</v>
       </c>
-      <c r="U47" s="30">
+      <c r="U48" s="30">
         <v>3218</v>
       </c>
-      <c r="V47" s="30">
+      <c r="V48" s="30">
         <v>5319</v>
       </c>
-      <c r="W47" s="30">
+      <c r="W48" s="30">
         <v>6871</v>
       </c>
-      <c r="X47" s="31">
+      <c r="X48" s="31">
         <v>18549</v>
       </c>
-      <c r="Y47" s="31">
+      <c r="Y48" s="31">
         <v>-4533</v>
       </c>
-      <c r="Z47" s="31">
+      <c r="Z48" s="31">
         <v>16327</v>
       </c>
-      <c r="AA47" s="31">
+      <c r="AA48" s="31">
         <v>11032</v>
       </c>
-      <c r="AB47" s="31">
+      <c r="AB48" s="31">
         <v>6902</v>
       </c>
-      <c r="AC47" s="31">
+      <c r="AC48" s="31">
         <v>-5193</v>
       </c>
-      <c r="AD47" s="31">
+      <c r="AD48" s="31">
         <v>1144</v>
       </c>
-      <c r="AE47" s="8">
+      <c r="AE48" s="8">
         <v>6746</v>
       </c>
-      <c r="AF47" s="8">
+      <c r="AF48" s="8">
         <v>13945</v>
       </c>
-      <c r="AG47" s="8">
+      <c r="AG48" s="8">
         <v>2369</v>
       </c>
-      <c r="AH47" s="8">
+      <c r="AH48" s="8">
         <v>5456</v>
       </c>
-      <c r="AI47" s="8">
+      <c r="AI48" s="8">
         <v>7200</v>
       </c>
-    </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B48" s="27" t="s">
+      <c r="AJ48" s="8">
+        <v>5945</v>
+      </c>
+    </row>
+    <row r="49" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B49" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="39">
+      <c r="C49" s="27"/>
+      <c r="D49" s="35">
         <v>466</v>
       </c>
-      <c r="E48" s="39">
+      <c r="E49" s="35">
         <v>632</v>
       </c>
-      <c r="F48" s="39">
+      <c r="F49" s="35">
         <v>477</v>
       </c>
-      <c r="G48" s="39">
+      <c r="G49" s="35">
         <v>483</v>
       </c>
-      <c r="H48" s="39">
+      <c r="H49" s="35">
         <v>545</v>
       </c>
-      <c r="I48" s="39">
+      <c r="I49" s="35">
         <v>558</v>
       </c>
-      <c r="J48" s="39">
+      <c r="J49" s="35">
         <v>562</v>
       </c>
-      <c r="K48" s="39">
+      <c r="K49" s="35">
         <v>415</v>
       </c>
-      <c r="L48" s="39">
+      <c r="L49" s="35">
         <v>444</v>
       </c>
-      <c r="M48" s="39">
+      <c r="M49" s="35">
         <v>650</v>
       </c>
-      <c r="N48" s="39">
+      <c r="N49" s="35">
         <v>469</v>
       </c>
-      <c r="O48" s="39">
+      <c r="O49" s="35">
         <v>451</v>
       </c>
-      <c r="P48" s="39">
+      <c r="P49" s="35">
         <v>557</v>
       </c>
-      <c r="Q48" s="39">
+      <c r="Q49" s="35">
         <v>574</v>
       </c>
-      <c r="R48" s="39">
+      <c r="R49" s="35">
         <v>568</v>
       </c>
-      <c r="S48" s="39">
+      <c r="S49" s="35">
         <v>562</v>
       </c>
-      <c r="T48" s="39">
+      <c r="T49" s="35">
         <v>629</v>
       </c>
-      <c r="U48" s="39">
+      <c r="U49" s="35">
         <v>695</v>
       </c>
-      <c r="V48" s="39">
+      <c r="V49" s="35">
         <v>555</v>
       </c>
-      <c r="W48" s="39">
+      <c r="W49" s="35">
         <v>657</v>
       </c>
-      <c r="X48" s="39">
+      <c r="X49" s="35">
         <v>724</v>
       </c>
-      <c r="Y48" s="39">
+      <c r="Y49" s="35">
         <v>866</v>
       </c>
-      <c r="Z48" s="39">
+      <c r="Z49" s="35">
         <v>760</v>
       </c>
-      <c r="AA48" s="39">
+      <c r="AA49" s="35">
         <v>829</v>
       </c>
-      <c r="AB48" s="39">
+      <c r="AB49" s="35">
         <v>838</v>
       </c>
-      <c r="AC48" s="39">
+      <c r="AC49" s="35">
         <v>959</v>
       </c>
-      <c r="AD48" s="39">
+      <c r="AD49" s="35">
         <v>743</v>
       </c>
-      <c r="AE48" s="39">
+      <c r="AE49" s="35">
         <v>853</v>
       </c>
-      <c r="AF48" s="39">
+      <c r="AF49" s="35">
         <v>991</v>
       </c>
-      <c r="AG48" s="39">
+      <c r="AG49" s="35">
         <v>912</v>
       </c>
-      <c r="AH48" s="39">
+      <c r="AH49" s="35">
         <v>898</v>
       </c>
-      <c r="AI48" s="27">
+      <c r="AI49" s="27">
         <v>886</v>
       </c>
-    </row>
-    <row r="49" spans="2:44" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="30" t="s">
+      <c r="AJ49" s="1">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="50" spans="2:44" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="8">
-        <f t="shared" ref="D49:Q49" si="14">D47-D48</f>
+      <c r="D50" s="8">
+        <f t="shared" ref="D50:Q50" si="16">D48-D49</f>
         <v>7080</v>
       </c>
-      <c r="E49" s="8">
-        <f t="shared" si="14"/>
+      <c r="E50" s="8">
+        <f t="shared" si="16"/>
         <v>-3209</v>
       </c>
-      <c r="F49" s="8">
-        <f t="shared" si="14"/>
+      <c r="F50" s="8">
+        <f t="shared" si="16"/>
         <v>7892</v>
       </c>
-      <c r="G49" s="8">
-        <f t="shared" si="14"/>
+      <c r="G50" s="8">
+        <f t="shared" si="16"/>
         <v>3524</v>
       </c>
-      <c r="H49" s="8">
-        <f t="shared" si="14"/>
+      <c r="H50" s="8">
+        <f t="shared" si="16"/>
         <v>396</v>
       </c>
-      <c r="I49" s="8">
-        <f t="shared" si="14"/>
+      <c r="I50" s="8">
+        <f t="shared" si="16"/>
         <v>1838</v>
       </c>
-      <c r="J49" s="8">
-        <f t="shared" si="14"/>
+      <c r="J50" s="8">
+        <f t="shared" si="16"/>
         <v>2672</v>
       </c>
-      <c r="K49" s="8">
-        <f t="shared" si="14"/>
+      <c r="K50" s="8">
+        <f t="shared" si="16"/>
         <v>5459</v>
       </c>
-      <c r="L49" s="8">
-        <f t="shared" si="14"/>
+      <c r="L50" s="8">
+        <f t="shared" si="16"/>
         <v>2706</v>
       </c>
-      <c r="M49" s="8">
-        <f t="shared" si="14"/>
+      <c r="M50" s="8">
+        <f t="shared" si="16"/>
         <v>5555</v>
       </c>
-      <c r="N49" s="8">
-        <f t="shared" si="14"/>
+      <c r="N50" s="8">
+        <f t="shared" si="16"/>
         <v>2474</v>
       </c>
-      <c r="O49" s="8">
-        <f t="shared" si="14"/>
+      <c r="O50" s="8">
+        <f t="shared" si="16"/>
         <v>9552</v>
       </c>
-      <c r="P49" s="8">
-        <f t="shared" si="14"/>
+      <c r="P50" s="8">
+        <f t="shared" si="16"/>
         <v>2570</v>
       </c>
-      <c r="Q49" s="8">
-        <f t="shared" si="14"/>
+      <c r="Q50" s="8">
+        <f t="shared" si="16"/>
         <v>5527</v>
       </c>
-      <c r="R49" s="8">
-        <f t="shared" ref="R49:AI49" si="15">R47-R48</f>
+      <c r="R50" s="8">
+        <f t="shared" ref="R50:AI50" si="17">R48-R49</f>
         <v>5437</v>
       </c>
-      <c r="S49" s="8">
-        <f t="shared" si="15"/>
+      <c r="S50" s="8">
+        <f t="shared" si="17"/>
         <v>4978</v>
       </c>
-      <c r="T49" s="8">
-        <f t="shared" si="15"/>
+      <c r="T50" s="8">
+        <f t="shared" si="17"/>
         <v>6951</v>
       </c>
-      <c r="U49" s="8">
-        <f t="shared" si="15"/>
+      <c r="U50" s="8">
+        <f t="shared" si="17"/>
         <v>2523</v>
       </c>
-      <c r="V49" s="8">
-        <f t="shared" si="15"/>
+      <c r="V50" s="8">
+        <f t="shared" si="17"/>
         <v>4764</v>
       </c>
-      <c r="W49" s="8">
-        <f t="shared" si="15"/>
+      <c r="W50" s="8">
+        <f t="shared" si="17"/>
         <v>6214</v>
       </c>
-      <c r="X49" s="8">
-        <f t="shared" si="15"/>
+      <c r="X50" s="8">
+        <f t="shared" si="17"/>
         <v>17825</v>
       </c>
-      <c r="Y49" s="8">
-        <f t="shared" si="15"/>
+      <c r="Y50" s="8">
+        <f t="shared" si="17"/>
         <v>-5399</v>
       </c>
-      <c r="Z49" s="8">
-        <f t="shared" si="15"/>
+      <c r="Z50" s="8">
+        <f t="shared" si="17"/>
         <v>15567</v>
       </c>
-      <c r="AA49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AA50" s="8">
+        <f t="shared" si="17"/>
         <v>10203</v>
       </c>
-      <c r="AB49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AB50" s="8">
+        <f t="shared" si="17"/>
         <v>6064</v>
       </c>
-      <c r="AC49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AC50" s="8">
+        <f t="shared" si="17"/>
         <v>-6152</v>
       </c>
-      <c r="AD49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AD50" s="8">
+        <f t="shared" si="17"/>
         <v>401</v>
       </c>
-      <c r="AE49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AE50" s="8">
+        <f t="shared" si="17"/>
         <v>5893</v>
       </c>
-      <c r="AF49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AF50" s="8">
+        <f t="shared" si="17"/>
         <v>12954</v>
       </c>
-      <c r="AG49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AG50" s="8">
+        <f t="shared" si="17"/>
         <v>1457</v>
       </c>
-      <c r="AH49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AH50" s="8">
+        <f t="shared" si="17"/>
         <v>4558</v>
       </c>
-      <c r="AI49" s="8">
-        <f t="shared" si="15"/>
+      <c r="AI50" s="8">
+        <f t="shared" si="17"/>
         <v>6314</v>
       </c>
-      <c r="AJ49" s="8">
-        <f>AJ47-AJ48</f>
+      <c r="AJ50" s="8">
+        <f>AJ48-AJ49</f>
+        <v>5055</v>
+      </c>
+      <c r="AK50" s="8">
+        <f>AK48-AK49</f>
         <v>0</v>
       </c>
-      <c r="AK49" s="8">
-        <f>AK47-AK48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
-      <c r="X50" s="28"/>
-      <c r="Y50" s="28"/>
-      <c r="Z50" s="28"/>
-      <c r="AA50" s="28"/>
-      <c r="AB50" s="28"/>
-      <c r="AC50" s="28"/>
-      <c r="AD50" s="28"/>
     </row>
     <row r="51" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="27"/>
+      <c r="X51" s="28"/>
+      <c r="Y51" s="28"/>
+      <c r="Z51" s="28"/>
+      <c r="AA51" s="28"/>
+      <c r="AB51" s="28"/>
+      <c r="AC51" s="28"/>
+      <c r="AD51" s="28"/>
+    </row>
+    <row r="52" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B52" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="G52" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H51" s="6">
-        <f t="shared" ref="H51" si="16">IF(D49=0,IF(H49=0,0,NA()),(H49-D49)/ABS(D49))</f>
+      <c r="H52" s="6">
+        <f t="shared" ref="H52" si="18">IF(D50=0,IF(H50=0,0,NA()),(H50-D50)/ABS(D50))</f>
         <v>-0.94406779661016949</v>
       </c>
-      <c r="I51" s="6">
-        <f t="shared" ref="I51" si="17">IF(E49=0,IF(I49=0,0,NA()),(I49-E49)/ABS(E49))</f>
+      <c r="I52" s="6">
+        <f t="shared" ref="I52" si="19">IF(E50=0,IF(I50=0,0,NA()),(I50-E50)/ABS(E50))</f>
         <v>1.5727641009660331</v>
       </c>
-      <c r="J51" s="6">
-        <f t="shared" ref="J51" si="18">IF(F49=0,IF(J49=0,0,NA()),(J49-F49)/ABS(F49))</f>
+      <c r="J52" s="6">
+        <f t="shared" ref="J52" si="20">IF(F50=0,IF(J50=0,0,NA()),(J50-F50)/ABS(F50))</f>
         <v>-0.6614292954891029</v>
       </c>
-      <c r="K51" s="6">
-        <f t="shared" ref="K51" si="19">IF(G49=0,IF(K49=0,0,NA()),(K49-G49)/ABS(G49))</f>
+      <c r="K52" s="6">
+        <f t="shared" ref="K52" si="21">IF(G50=0,IF(K50=0,0,NA()),(K50-G50)/ABS(G50))</f>
         <v>0.54909194097616343</v>
       </c>
-      <c r="L51" s="6">
-        <f t="shared" ref="L51" si="20">IF(H49=0,IF(L49=0,0,NA()),(L49-H49)/ABS(H49))</f>
+      <c r="L52" s="6">
+        <f t="shared" ref="L52" si="22">IF(H50=0,IF(L50=0,0,NA()),(L50-H50)/ABS(H50))</f>
         <v>5.833333333333333</v>
       </c>
-      <c r="M51" s="6">
-        <f t="shared" ref="M51" si="21">IF(I49=0,IF(M49=0,0,NA()),(M49-I49)/ABS(I49))</f>
+      <c r="M52" s="6">
+        <f t="shared" ref="M52" si="23">IF(I50=0,IF(M50=0,0,NA()),(M50-I50)/ABS(I50))</f>
         <v>2.0223068552774754</v>
       </c>
-      <c r="N51" s="6">
-        <f t="shared" ref="N51" si="22">IF(J49=0,IF(N49=0,0,NA()),(N49-J49)/ABS(J49))</f>
+      <c r="N52" s="6">
+        <f t="shared" ref="N52" si="24">IF(J50=0,IF(N50=0,0,NA()),(N50-J50)/ABS(J50))</f>
         <v>-7.410179640718563E-2</v>
       </c>
-      <c r="O51" s="6">
-        <f t="shared" ref="O51" si="23">IF(K49=0,IF(O49=0,0,NA()),(O49-K49)/ABS(K49))</f>
+      <c r="O52" s="6">
+        <f t="shared" ref="O52" si="25">IF(K50=0,IF(O50=0,0,NA()),(O50-K50)/ABS(K50))</f>
         <v>0.74977102033339438</v>
       </c>
-      <c r="P51" s="6">
-        <f t="shared" ref="P51" si="24">IF(L49=0,IF(P49=0,0,NA()),(P49-L49)/ABS(L49))</f>
+      <c r="P52" s="6">
+        <f t="shared" ref="P52" si="26">IF(L50=0,IF(P50=0,0,NA()),(P50-L50)/ABS(L50))</f>
         <v>-5.0258684405025872E-2</v>
       </c>
-      <c r="Q51" s="6">
-        <f t="shared" ref="Q51" si="25">IF(M49=0,IF(Q49=0,0,NA()),(Q49-M49)/ABS(M49))</f>
+      <c r="Q52" s="6">
+        <f t="shared" ref="Q52" si="27">IF(M50=0,IF(Q50=0,0,NA()),(Q50-M50)/ABS(M50))</f>
         <v>-5.0405040504050407E-3</v>
       </c>
-      <c r="R51" s="6">
-        <f t="shared" ref="R51" si="26">IF(N49=0,IF(R49=0,0,NA()),(R49-N49)/ABS(N49))</f>
+      <c r="R52" s="6">
+        <f t="shared" ref="R52" si="28">IF(N50=0,IF(R50=0,0,NA()),(R50-N50)/ABS(N50))</f>
         <v>1.1976556184316896</v>
       </c>
-      <c r="S51" s="6">
-        <f t="shared" ref="S51" si="27">IF(O49=0,IF(S49=0,0,NA()),(S49-O49)/ABS(O49))</f>
+      <c r="S52" s="6">
+        <f t="shared" ref="S52" si="29">IF(O50=0,IF(S50=0,0,NA()),(S50-O50)/ABS(O50))</f>
         <v>-0.4788525963149079</v>
       </c>
-      <c r="T51" s="6">
-        <f t="shared" ref="T51" si="28">IF(P49=0,IF(T49=0,0,NA()),(T49-P49)/ABS(P49))</f>
+      <c r="T52" s="6">
+        <f t="shared" ref="T52" si="30">IF(P50=0,IF(T50=0,0,NA()),(T50-P50)/ABS(P50))</f>
         <v>1.704669260700389</v>
       </c>
-      <c r="U51" s="6">
-        <f t="shared" ref="U51" si="29">IF(Q49=0,IF(U49=0,0,NA()),(U49-Q49)/ABS(Q49))</f>
+      <c r="U52" s="6">
+        <f t="shared" ref="U52" si="31">IF(Q50=0,IF(U50=0,0,NA()),(U50-Q50)/ABS(Q50))</f>
         <v>-0.54351366021349734</v>
       </c>
-      <c r="V51" s="6">
-        <f t="shared" ref="V51" si="30">IF(R49=0,IF(V49=0,0,NA()),(V49-R49)/ABS(R49))</f>
+      <c r="V52" s="6">
+        <f t="shared" ref="V52" si="32">IF(R50=0,IF(V50=0,0,NA()),(V50-R50)/ABS(R50))</f>
         <v>-0.12378149714916314</v>
       </c>
-      <c r="W51" s="6">
-        <f t="shared" ref="W51" si="31">IF(S49=0,IF(W49=0,0,NA()),(W49-S49)/ABS(S49))</f>
+      <c r="W52" s="6">
+        <f t="shared" ref="W52" si="33">IF(S50=0,IF(W50=0,0,NA()),(W50-S50)/ABS(S50))</f>
         <v>0.24829248694254721</v>
       </c>
-      <c r="X51" s="6">
-        <f t="shared" ref="X51" si="32">IF(T49=0,IF(X49=0,0,NA()),(X49-T49)/ABS(T49))</f>
+      <c r="X52" s="6">
+        <f t="shared" ref="X52" si="34">IF(T50=0,IF(X50=0,0,NA()),(X50-T50)/ABS(T50))</f>
         <v>1.5643792260106459</v>
       </c>
-      <c r="Y51" s="6">
-        <f t="shared" ref="Y51" si="33">IF(U49=0,IF(Y49=0,0,NA()),(Y49-U49)/ABS(U49))</f>
+      <c r="Y52" s="6">
+        <f t="shared" ref="Y52" si="35">IF(U50=0,IF(Y50=0,0,NA()),(Y50-U50)/ABS(U50))</f>
         <v>-3.1399128022195799</v>
       </c>
-      <c r="Z51" s="6">
-        <f t="shared" ref="Z51:AG51" si="34">IF(V49=0,IF(Z49=0,0,NA()),(Z49-V49)/ABS(V49))</f>
+      <c r="Z52" s="6">
+        <f t="shared" ref="Z52:AG52" si="36">IF(V50=0,IF(Z50=0,0,NA()),(Z50-V50)/ABS(V50))</f>
         <v>2.2676322418136019</v>
       </c>
-      <c r="AA51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AA52" s="6">
+        <f t="shared" si="36"/>
         <v>0.64193756034760219</v>
       </c>
-      <c r="AB51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AB52" s="6">
+        <f t="shared" si="36"/>
         <v>-0.65980364656381485</v>
       </c>
-      <c r="AC51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AC52" s="6">
+        <f t="shared" si="36"/>
         <v>-0.13947027227264308</v>
       </c>
-      <c r="AD51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AD52" s="6">
+        <f t="shared" si="36"/>
         <v>-0.97424038029164262</v>
       </c>
-      <c r="AE51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AE52" s="6">
+        <f t="shared" si="36"/>
         <v>-0.42242477702636477</v>
       </c>
-      <c r="AF51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AF52" s="6">
+        <f t="shared" si="36"/>
         <v>1.1362137203166227</v>
       </c>
-      <c r="AG51" s="6">
-        <f t="shared" si="34"/>
+      <c r="AG52" s="6">
+        <f t="shared" si="36"/>
         <v>1.2368335500650196</v>
       </c>
-      <c r="AH51" s="6">
-        <f>IF(AD49=0,IF(AH49=0,0,NA()),(AH49-AD49)/ABS(AD49))</f>
+      <c r="AH52" s="6">
+        <f>IF(AD50=0,IF(AH50=0,0,NA()),(AH50-AD50)/ABS(AD50))</f>
         <v>10.366583541147133</v>
       </c>
-      <c r="AI51" s="6">
-        <f>IF(AE49=0,IF(AI49=0,0,NA()),(AI49-AE49)/ABS(AE49))</f>
+      <c r="AI52" s="6">
+        <f t="shared" ref="AI52:AJ52" si="37">IF(AE50=0,IF(AI50=0,0,NA()),(AI50-AE50)/ABS(AE50))</f>
         <v>7.14406923468522E-2</v>
       </c>
-    </row>
-    <row r="53" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="27"/>
-      <c r="Y53" s="10"/>
-    </row>
-    <row r="54" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B54" s="11" t="s">
+      <c r="AJ52" s="6">
+        <f t="shared" si="37"/>
+        <v>-0.60977304307549796</v>
+      </c>
+    </row>
+    <row r="54" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="27"/>
+      <c r="Y54" s="10"/>
+    </row>
+    <row r="55" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B55" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="12"/>
-      <c r="S54" s="12"/>
-      <c r="T54" s="12"/>
-      <c r="U54" s="12"/>
-      <c r="V54" s="12"/>
-      <c r="W54" s="12"/>
-      <c r="X54" s="12"/>
-      <c r="Y54" s="12"/>
-      <c r="Z54" s="12"/>
-      <c r="AA54" s="12"/>
-      <c r="AB54" s="12"/>
-      <c r="AC54" s="12"/>
-      <c r="AD54" s="12"/>
-      <c r="AE54" s="12"/>
-      <c r="AF54" s="12"/>
-      <c r="AG54" s="12"/>
-      <c r="AI54" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ54" s="12"/>
-      <c r="AK54" s="12"/>
-      <c r="AL54" s="12"/>
-      <c r="AM54" s="12"/>
-      <c r="AN54" s="12"/>
-      <c r="AO54" s="12"/>
-      <c r="AP54" s="12"/>
-      <c r="AQ54" s="12"/>
-      <c r="AR54" s="14"/>
-    </row>
-    <row r="55" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="AI55" s="1" t="s">
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="12"/>
+      <c r="U55" s="12"/>
+      <c r="V55" s="12"/>
+      <c r="W55" s="12"/>
+      <c r="X55" s="12"/>
+      <c r="Y55" s="12"/>
+      <c r="Z55" s="12"/>
+      <c r="AA55" s="12"/>
+      <c r="AB55" s="12"/>
+      <c r="AC55" s="12"/>
+      <c r="AD55" s="12"/>
+      <c r="AE55" s="12"/>
+      <c r="AF55" s="12"/>
+      <c r="AG55" s="12"/>
+      <c r="AI55" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="AR55" s="16"/>
+      <c r="AJ55" s="12"/>
+      <c r="AK55" s="12"/>
+      <c r="AL55" s="12"/>
+      <c r="AM55" s="12"/>
+      <c r="AN55" s="12"/>
+      <c r="AO55" s="12"/>
+      <c r="AP55" s="12"/>
+      <c r="AQ55" s="12"/>
+      <c r="AR55" s="14"/>
     </row>
     <row r="56" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B56" s="15"/>
-      <c r="AI56" s="17"/>
+      <c r="AJ56" s="38" t="s">
+        <v>117</v>
+      </c>
       <c r="AR56" s="16"/>
     </row>
-    <row r="57" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="19"/>
-      <c r="O57" s="19"/>
-      <c r="P57" s="19"/>
-      <c r="Q57" s="19"/>
-      <c r="R57" s="19"/>
-      <c r="S57" s="19"/>
-      <c r="T57" s="19"/>
-      <c r="U57" s="19"/>
-      <c r="V57" s="19"/>
-      <c r="W57" s="19"/>
-      <c r="X57" s="19"/>
-      <c r="Y57" s="19"/>
-      <c r="Z57" s="19"/>
-      <c r="AA57" s="19"/>
-      <c r="AB57" s="19"/>
-      <c r="AC57" s="19"/>
-      <c r="AD57" s="19"/>
-      <c r="AE57" s="19"/>
-      <c r="AF57" s="19"/>
-      <c r="AG57" s="19"/>
-      <c r="AH57" s="19"/>
-      <c r="AI57" s="19"/>
-      <c r="AJ57" s="19"/>
-      <c r="AK57" s="19"/>
-      <c r="AL57" s="19"/>
-      <c r="AM57" s="19"/>
-      <c r="AN57" s="19"/>
-      <c r="AO57" s="19"/>
-      <c r="AP57" s="19"/>
-      <c r="AQ57" s="19"/>
-      <c r="AR57" s="20"/>
-    </row>
-    <row r="58" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B59" s="11" t="s">
+    <row r="57" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="AI57" s="17"/>
+      <c r="AR57" s="16"/>
+    </row>
+    <row r="58" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="19"/>
+      <c r="S58" s="19"/>
+      <c r="T58" s="19"/>
+      <c r="U58" s="19"/>
+      <c r="V58" s="19"/>
+      <c r="W58" s="19"/>
+      <c r="X58" s="19"/>
+      <c r="Y58" s="19"/>
+      <c r="Z58" s="19"/>
+      <c r="AA58" s="19"/>
+      <c r="AB58" s="19"/>
+      <c r="AC58" s="19"/>
+      <c r="AD58" s="19"/>
+      <c r="AE58" s="19"/>
+      <c r="AF58" s="19"/>
+      <c r="AG58" s="19"/>
+      <c r="AH58" s="19"/>
+      <c r="AI58" s="19"/>
+      <c r="AJ58" s="19"/>
+      <c r="AK58" s="19"/>
+      <c r="AL58" s="19"/>
+      <c r="AM58" s="19"/>
+      <c r="AN58" s="19"/>
+      <c r="AO58" s="19"/>
+      <c r="AP58" s="19"/>
+      <c r="AQ58" s="19"/>
+      <c r="AR58" s="20"/>
+    </row>
+    <row r="59" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B60" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="12"/>
-      <c r="S59" s="12"/>
-      <c r="T59" s="12"/>
-      <c r="U59" s="12"/>
-      <c r="V59" s="12"/>
-      <c r="W59" s="12"/>
-      <c r="X59" s="12"/>
-      <c r="Y59" s="12"/>
-      <c r="Z59" s="12"/>
-      <c r="AA59" s="12"/>
-      <c r="AC59" s="12"/>
-      <c r="AD59" s="12"/>
-      <c r="AE59" s="12"/>
-      <c r="AF59" s="12"/>
-      <c r="AG59" s="12"/>
-    </row>
-    <row r="60" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="12"/>
+      <c r="T60" s="12"/>
+      <c r="U60" s="12"/>
+      <c r="V60" s="12"/>
+      <c r="W60" s="12"/>
+      <c r="X60" s="12"/>
+      <c r="Y60" s="12"/>
+      <c r="Z60" s="12"/>
+      <c r="AA60" s="12"/>
+      <c r="AC60" s="12"/>
+      <c r="AD60" s="12"/>
+      <c r="AE60" s="12"/>
+      <c r="AF60" s="12"/>
+      <c r="AG60" s="12"/>
     </row>
     <row r="61" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B61" s="15"/>
-      <c r="R61" s="27"/>
-      <c r="S61" s="27"/>
-      <c r="T61" s="27"/>
-      <c r="U61" s="27"/>
-      <c r="V61" s="27"/>
-      <c r="W61" s="27"/>
-      <c r="X61" s="28"/>
-      <c r="Y61" s="28"/>
-      <c r="Z61" s="28"/>
-      <c r="AA61" s="28"/>
-      <c r="AB61" s="28"/>
-      <c r="AC61" s="28"/>
-      <c r="AD61" s="28"/>
-      <c r="AE61" s="28"/>
-      <c r="AG61" s="9"/>
     </row>
     <row r="62" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B62" s="15"/>
-    </row>
-    <row r="63" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="19"/>
-      <c r="P63" s="19"/>
-      <c r="Q63" s="19"/>
-      <c r="R63" s="19"/>
-      <c r="S63" s="19"/>
-      <c r="T63" s="19"/>
-      <c r="U63" s="19"/>
-      <c r="V63" s="19"/>
-      <c r="W63" s="19"/>
-      <c r="X63" s="19"/>
-      <c r="Y63" s="19"/>
-      <c r="Z63" s="19"/>
-      <c r="AA63" s="19"/>
-      <c r="AB63" s="19"/>
-      <c r="AC63" s="19"/>
-      <c r="AD63" s="19"/>
-      <c r="AE63" s="19"/>
-      <c r="AF63" s="19"/>
-      <c r="AG63" s="19"/>
-    </row>
-    <row r="64" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="35"/>
-      <c r="P65" s="35"/>
-      <c r="Q65" s="35"/>
-    </row>
+      <c r="R62" s="27"/>
+      <c r="S62" s="27"/>
+      <c r="T62" s="27"/>
+      <c r="U62" s="27"/>
+      <c r="V62" s="27"/>
+      <c r="W62" s="27"/>
+      <c r="X62" s="28"/>
+      <c r="Y62" s="28"/>
+      <c r="Z62" s="28"/>
+      <c r="AA62" s="28"/>
+      <c r="AB62" s="28"/>
+      <c r="AC62" s="28"/>
+      <c r="AD62" s="28"/>
+      <c r="AE62" s="28"/>
+      <c r="AG62" s="9"/>
+    </row>
+    <row r="63" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B63" s="15"/>
+    </row>
+    <row r="64" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="19"/>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="19"/>
+      <c r="S64" s="19"/>
+      <c r="T64" s="19"/>
+      <c r="U64" s="19"/>
+      <c r="V64" s="19"/>
+      <c r="W64" s="19"/>
+      <c r="X64" s="19"/>
+      <c r="Y64" s="19"/>
+      <c r="Z64" s="19"/>
+      <c r="AA64" s="19"/>
+      <c r="AB64" s="19"/>
+      <c r="AC64" s="19"/>
+      <c r="AD64" s="19"/>
+      <c r="AE64" s="19"/>
+      <c r="AF64" s="19"/>
+      <c r="AG64" s="19"/>
+    </row>
+    <row r="65" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B66" s="15"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="12"/>
     </row>
     <row r="67" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B67" s="15"/>
@@ -5852,531 +5934,516 @@
     <row r="68" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="35"/>
-      <c r="L69" s="35"/>
-      <c r="M69" s="35"/>
-      <c r="N69" s="35"/>
-      <c r="O69" s="35"/>
-      <c r="P69" s="35"/>
-      <c r="Q69" s="35"/>
-    </row>
-    <row r="70" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B71" s="11"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="12"/>
-      <c r="Q71" s="12"/>
-      <c r="R71" s="12"/>
-      <c r="S71" s="12"/>
-      <c r="T71" s="12"/>
-      <c r="U71" s="12"/>
-      <c r="V71" s="12"/>
-      <c r="W71" s="12"/>
-      <c r="X71" s="12"/>
-      <c r="Y71" s="12"/>
-      <c r="Z71" s="12"/>
-      <c r="AA71" s="12"/>
-      <c r="AB71" s="12"/>
-      <c r="AC71" s="12"/>
-      <c r="AD71" s="12"/>
-      <c r="AE71" s="12"/>
-      <c r="AF71" s="12"/>
-      <c r="AG71" s="12"/>
-      <c r="AH71" s="12"/>
-      <c r="AI71" s="12"/>
-      <c r="AJ71" s="12"/>
-      <c r="AK71" s="12"/>
-      <c r="AL71" s="12"/>
-      <c r="AM71" s="12"/>
-      <c r="AN71" s="12"/>
-      <c r="AO71" s="12"/>
-      <c r="AP71" s="12"/>
-      <c r="AQ71" s="12"/>
-      <c r="AR71" s="14"/>
-    </row>
+    <row r="69" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
+    </row>
+    <row r="71" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B72" s="15"/>
-      <c r="AR72" s="16"/>
-    </row>
-    <row r="73" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="11"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="12"/>
+      <c r="S72" s="12"/>
+      <c r="T72" s="12"/>
+      <c r="U72" s="12"/>
+      <c r="V72" s="12"/>
+      <c r="W72" s="12"/>
+      <c r="X72" s="12"/>
+      <c r="Y72" s="12"/>
+      <c r="Z72" s="12"/>
+      <c r="AA72" s="12"/>
+      <c r="AB72" s="12"/>
+      <c r="AC72" s="12"/>
+      <c r="AD72" s="12"/>
+      <c r="AE72" s="12"/>
+      <c r="AF72" s="12"/>
+      <c r="AG72" s="12"/>
+      <c r="AH72" s="12"/>
+      <c r="AI72" s="12"/>
+      <c r="AJ72" s="12"/>
+      <c r="AK72" s="12"/>
+      <c r="AL72" s="12"/>
+      <c r="AM72" s="12"/>
+      <c r="AN72" s="12"/>
+      <c r="AO72" s="12"/>
+      <c r="AP72" s="12"/>
+      <c r="AQ72" s="12"/>
+      <c r="AR72" s="14"/>
+    </row>
+    <row r="73" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B73" s="15"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="33"/>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="33"/>
-      <c r="L73" s="33"/>
-      <c r="M73" s="33"/>
-      <c r="N73" s="33"/>
-      <c r="O73" s="33"/>
-      <c r="P73" s="33"/>
-      <c r="Q73" s="33"/>
-      <c r="R73" s="33"/>
-      <c r="S73" s="33"/>
-      <c r="T73" s="33"/>
-      <c r="U73" s="33"/>
-      <c r="V73" s="33"/>
-      <c r="W73" s="33"/>
-      <c r="X73" s="33"/>
-      <c r="Y73" s="33"/>
-      <c r="Z73" s="33"/>
-      <c r="AA73" s="33"/>
-      <c r="AB73" s="33"/>
-      <c r="AC73" s="33"/>
-      <c r="AD73" s="33"/>
-      <c r="AE73" s="33"/>
-      <c r="AF73" s="33"/>
-      <c r="AG73" s="33"/>
-      <c r="AH73" s="33"/>
-      <c r="AI73" s="33"/>
-      <c r="AJ73" s="33"/>
-      <c r="AK73" s="33"/>
-      <c r="AL73" s="33"/>
-      <c r="AM73" s="33"/>
-      <c r="AN73" s="33"/>
-      <c r="AO73" s="33"/>
-      <c r="AP73" s="33"/>
-      <c r="AQ73" s="33"/>
-      <c r="AR73" s="34"/>
+      <c r="AR73" s="16"/>
     </row>
     <row r="74" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="15"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="33"/>
-      <c r="I74" s="33"/>
-      <c r="J74" s="33"/>
-      <c r="K74" s="33"/>
-      <c r="L74" s="33"/>
-      <c r="M74" s="33"/>
-      <c r="N74" s="33"/>
-      <c r="O74" s="33"/>
-      <c r="P74" s="33"/>
-      <c r="Q74" s="33"/>
-      <c r="R74" s="33"/>
-      <c r="S74" s="33"/>
-      <c r="T74" s="33"/>
-      <c r="U74" s="33"/>
-      <c r="V74" s="33"/>
-      <c r="W74" s="33"/>
-      <c r="X74" s="33"/>
-      <c r="Y74" s="33"/>
-      <c r="Z74" s="33"/>
-      <c r="AA74" s="33"/>
-      <c r="AB74" s="33"/>
-      <c r="AC74" s="33"/>
-      <c r="AD74" s="33"/>
-      <c r="AE74" s="33"/>
-      <c r="AF74" s="33"/>
-      <c r="AG74" s="33"/>
-      <c r="AH74" s="33"/>
-      <c r="AI74" s="33"/>
-      <c r="AJ74" s="33"/>
-      <c r="AK74" s="33"/>
-      <c r="AL74" s="33"/>
-      <c r="AM74" s="33"/>
-      <c r="AN74" s="33"/>
-      <c r="AO74" s="33"/>
-      <c r="AP74" s="33"/>
-      <c r="AQ74" s="33"/>
-      <c r="AR74" s="34"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="36"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
+      <c r="M74" s="36"/>
+      <c r="N74" s="36"/>
+      <c r="O74" s="36"/>
+      <c r="P74" s="36"/>
+      <c r="Q74" s="36"/>
+      <c r="R74" s="36"/>
+      <c r="S74" s="36"/>
+      <c r="T74" s="36"/>
+      <c r="U74" s="36"/>
+      <c r="V74" s="36"/>
+      <c r="W74" s="36"/>
+      <c r="X74" s="36"/>
+      <c r="Y74" s="36"/>
+      <c r="Z74" s="36"/>
+      <c r="AA74" s="36"/>
+      <c r="AB74" s="36"/>
+      <c r="AC74" s="36"/>
+      <c r="AD74" s="36"/>
+      <c r="AE74" s="36"/>
+      <c r="AF74" s="36"/>
+      <c r="AG74" s="36"/>
+      <c r="AH74" s="36"/>
+      <c r="AI74" s="36"/>
+      <c r="AJ74" s="36"/>
+      <c r="AK74" s="36"/>
+      <c r="AL74" s="36"/>
+      <c r="AM74" s="36"/>
+      <c r="AN74" s="36"/>
+      <c r="AO74" s="36"/>
+      <c r="AP74" s="36"/>
+      <c r="AQ74" s="36"/>
+      <c r="AR74" s="37"/>
     </row>
     <row r="75" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="15"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
-      <c r="L75" s="33"/>
-      <c r="M75" s="33"/>
-      <c r="N75" s="33"/>
-      <c r="O75" s="33"/>
-      <c r="P75" s="33"/>
-      <c r="Q75" s="33"/>
-      <c r="R75" s="33"/>
-      <c r="S75" s="33"/>
-      <c r="T75" s="33"/>
-      <c r="U75" s="33"/>
-      <c r="V75" s="33"/>
-      <c r="W75" s="33"/>
-      <c r="X75" s="33"/>
-      <c r="Y75" s="33"/>
-      <c r="Z75" s="33"/>
-      <c r="AA75" s="33"/>
-      <c r="AB75" s="33"/>
-      <c r="AC75" s="33"/>
-      <c r="AD75" s="33"/>
-      <c r="AE75" s="33"/>
-      <c r="AF75" s="33"/>
-      <c r="AG75" s="33"/>
-      <c r="AH75" s="33"/>
-      <c r="AI75" s="33"/>
-      <c r="AJ75" s="33"/>
-      <c r="AK75" s="33"/>
-      <c r="AL75" s="33"/>
-      <c r="AM75" s="33"/>
-      <c r="AN75" s="33"/>
-      <c r="AO75" s="33"/>
-      <c r="AP75" s="33"/>
-      <c r="AQ75" s="33"/>
-      <c r="AR75" s="34"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="36"/>
+      <c r="I75" s="36"/>
+      <c r="J75" s="36"/>
+      <c r="K75" s="36"/>
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+      <c r="N75" s="36"/>
+      <c r="O75" s="36"/>
+      <c r="P75" s="36"/>
+      <c r="Q75" s="36"/>
+      <c r="R75" s="36"/>
+      <c r="S75" s="36"/>
+      <c r="T75" s="36"/>
+      <c r="U75" s="36"/>
+      <c r="V75" s="36"/>
+      <c r="W75" s="36"/>
+      <c r="X75" s="36"/>
+      <c r="Y75" s="36"/>
+      <c r="Z75" s="36"/>
+      <c r="AA75" s="36"/>
+      <c r="AB75" s="36"/>
+      <c r="AC75" s="36"/>
+      <c r="AD75" s="36"/>
+      <c r="AE75" s="36"/>
+      <c r="AF75" s="36"/>
+      <c r="AG75" s="36"/>
+      <c r="AH75" s="36"/>
+      <c r="AI75" s="36"/>
+      <c r="AJ75" s="36"/>
+      <c r="AK75" s="36"/>
+      <c r="AL75" s="36"/>
+      <c r="AM75" s="36"/>
+      <c r="AN75" s="36"/>
+      <c r="AO75" s="36"/>
+      <c r="AP75" s="36"/>
+      <c r="AQ75" s="36"/>
+      <c r="AR75" s="37"/>
     </row>
     <row r="76" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="15"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
-      <c r="L76" s="33"/>
-      <c r="M76" s="33"/>
-      <c r="N76" s="33"/>
-      <c r="O76" s="33"/>
-      <c r="P76" s="33"/>
-      <c r="Q76" s="33"/>
-      <c r="R76" s="33"/>
-      <c r="S76" s="33"/>
-      <c r="T76" s="33"/>
-      <c r="U76" s="33"/>
-      <c r="V76" s="33"/>
-      <c r="W76" s="33"/>
-      <c r="X76" s="33"/>
-      <c r="Y76" s="33"/>
-      <c r="Z76" s="33"/>
-      <c r="AA76" s="33"/>
-      <c r="AB76" s="33"/>
-      <c r="AC76" s="33"/>
-      <c r="AD76" s="33"/>
-      <c r="AE76" s="33"/>
-      <c r="AF76" s="33"/>
-      <c r="AG76" s="33"/>
-      <c r="AH76" s="33"/>
-      <c r="AI76" s="33"/>
-      <c r="AJ76" s="33"/>
-      <c r="AK76" s="33"/>
-      <c r="AL76" s="33"/>
-      <c r="AM76" s="33"/>
-      <c r="AN76" s="33"/>
-      <c r="AO76" s="33"/>
-      <c r="AP76" s="33"/>
-      <c r="AQ76" s="33"/>
-      <c r="AR76" s="34"/>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="36"/>
+      <c r="I76" s="36"/>
+      <c r="J76" s="36"/>
+      <c r="K76" s="36"/>
+      <c r="L76" s="36"/>
+      <c r="M76" s="36"/>
+      <c r="N76" s="36"/>
+      <c r="O76" s="36"/>
+      <c r="P76" s="36"/>
+      <c r="Q76" s="36"/>
+      <c r="R76" s="36"/>
+      <c r="S76" s="36"/>
+      <c r="T76" s="36"/>
+      <c r="U76" s="36"/>
+      <c r="V76" s="36"/>
+      <c r="W76" s="36"/>
+      <c r="X76" s="36"/>
+      <c r="Y76" s="36"/>
+      <c r="Z76" s="36"/>
+      <c r="AA76" s="36"/>
+      <c r="AB76" s="36"/>
+      <c r="AC76" s="36"/>
+      <c r="AD76" s="36"/>
+      <c r="AE76" s="36"/>
+      <c r="AF76" s="36"/>
+      <c r="AG76" s="36"/>
+      <c r="AH76" s="36"/>
+      <c r="AI76" s="36"/>
+      <c r="AJ76" s="36"/>
+      <c r="AK76" s="36"/>
+      <c r="AL76" s="36"/>
+      <c r="AM76" s="36"/>
+      <c r="AN76" s="36"/>
+      <c r="AO76" s="36"/>
+      <c r="AP76" s="36"/>
+      <c r="AQ76" s="36"/>
+      <c r="AR76" s="37"/>
     </row>
     <row r="77" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="15"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
-      <c r="H77" s="33"/>
-      <c r="I77" s="33"/>
-      <c r="J77" s="33"/>
-      <c r="K77" s="33"/>
-      <c r="L77" s="33"/>
-      <c r="M77" s="33"/>
-      <c r="N77" s="33"/>
-      <c r="O77" s="33"/>
-      <c r="P77" s="33"/>
-      <c r="Q77" s="33"/>
-      <c r="R77" s="33"/>
-      <c r="S77" s="33"/>
-      <c r="T77" s="33"/>
-      <c r="U77" s="33"/>
-      <c r="V77" s="33"/>
-      <c r="W77" s="33"/>
-      <c r="X77" s="33"/>
-      <c r="Y77" s="33"/>
-      <c r="Z77" s="33"/>
-      <c r="AA77" s="33"/>
-      <c r="AB77" s="33"/>
-      <c r="AC77" s="33"/>
-      <c r="AD77" s="33"/>
-      <c r="AE77" s="33"/>
-      <c r="AF77" s="33"/>
-      <c r="AG77" s="33"/>
-      <c r="AH77" s="33"/>
-      <c r="AI77" s="33"/>
-      <c r="AJ77" s="33"/>
-      <c r="AK77" s="33"/>
-      <c r="AL77" s="33"/>
-      <c r="AM77" s="33"/>
-      <c r="AN77" s="33"/>
-      <c r="AO77" s="33"/>
-      <c r="AP77" s="33"/>
-      <c r="AQ77" s="33"/>
-      <c r="AR77" s="34"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
+      <c r="J77" s="36"/>
+      <c r="K77" s="36"/>
+      <c r="L77" s="36"/>
+      <c r="M77" s="36"/>
+      <c r="N77" s="36"/>
+      <c r="O77" s="36"/>
+      <c r="P77" s="36"/>
+      <c r="Q77" s="36"/>
+      <c r="R77" s="36"/>
+      <c r="S77" s="36"/>
+      <c r="T77" s="36"/>
+      <c r="U77" s="36"/>
+      <c r="V77" s="36"/>
+      <c r="W77" s="36"/>
+      <c r="X77" s="36"/>
+      <c r="Y77" s="36"/>
+      <c r="Z77" s="36"/>
+      <c r="AA77" s="36"/>
+      <c r="AB77" s="36"/>
+      <c r="AC77" s="36"/>
+      <c r="AD77" s="36"/>
+      <c r="AE77" s="36"/>
+      <c r="AF77" s="36"/>
+      <c r="AG77" s="36"/>
+      <c r="AH77" s="36"/>
+      <c r="AI77" s="36"/>
+      <c r="AJ77" s="36"/>
+      <c r="AK77" s="36"/>
+      <c r="AL77" s="36"/>
+      <c r="AM77" s="36"/>
+      <c r="AN77" s="36"/>
+      <c r="AO77" s="36"/>
+      <c r="AP77" s="36"/>
+      <c r="AQ77" s="36"/>
+      <c r="AR77" s="37"/>
     </row>
     <row r="78" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="15"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
-      <c r="H78" s="33"/>
-      <c r="I78" s="33"/>
-      <c r="J78" s="33"/>
-      <c r="K78" s="33"/>
-      <c r="L78" s="33"/>
-      <c r="M78" s="33"/>
-      <c r="N78" s="33"/>
-      <c r="O78" s="33"/>
-      <c r="P78" s="33"/>
-      <c r="Q78" s="33"/>
-      <c r="R78" s="33"/>
-      <c r="S78" s="33"/>
-      <c r="T78" s="33"/>
-      <c r="U78" s="33"/>
-      <c r="V78" s="33"/>
-      <c r="W78" s="33"/>
-      <c r="X78" s="33"/>
-      <c r="Y78" s="33"/>
-      <c r="Z78" s="33"/>
-      <c r="AA78" s="33"/>
-      <c r="AB78" s="33"/>
-      <c r="AC78" s="33"/>
-      <c r="AD78" s="33"/>
-      <c r="AE78" s="33"/>
-      <c r="AF78" s="33"/>
-      <c r="AG78" s="33"/>
-      <c r="AH78" s="33"/>
-      <c r="AI78" s="33"/>
-      <c r="AJ78" s="33"/>
-      <c r="AK78" s="33"/>
-      <c r="AL78" s="33"/>
-      <c r="AM78" s="33"/>
-      <c r="AN78" s="33"/>
-      <c r="AO78" s="33"/>
-      <c r="AP78" s="33"/>
-      <c r="AQ78" s="33"/>
-      <c r="AR78" s="34"/>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="36"/>
+      <c r="I78" s="36"/>
+      <c r="J78" s="36"/>
+      <c r="K78" s="36"/>
+      <c r="L78" s="36"/>
+      <c r="M78" s="36"/>
+      <c r="N78" s="36"/>
+      <c r="O78" s="36"/>
+      <c r="P78" s="36"/>
+      <c r="Q78" s="36"/>
+      <c r="R78" s="36"/>
+      <c r="S78" s="36"/>
+      <c r="T78" s="36"/>
+      <c r="U78" s="36"/>
+      <c r="V78" s="36"/>
+      <c r="W78" s="36"/>
+      <c r="X78" s="36"/>
+      <c r="Y78" s="36"/>
+      <c r="Z78" s="36"/>
+      <c r="AA78" s="36"/>
+      <c r="AB78" s="36"/>
+      <c r="AC78" s="36"/>
+      <c r="AD78" s="36"/>
+      <c r="AE78" s="36"/>
+      <c r="AF78" s="36"/>
+      <c r="AG78" s="36"/>
+      <c r="AH78" s="36"/>
+      <c r="AI78" s="36"/>
+      <c r="AJ78" s="36"/>
+      <c r="AK78" s="36"/>
+      <c r="AL78" s="36"/>
+      <c r="AM78" s="36"/>
+      <c r="AN78" s="36"/>
+      <c r="AO78" s="36"/>
+      <c r="AP78" s="36"/>
+      <c r="AQ78" s="36"/>
+      <c r="AR78" s="37"/>
     </row>
     <row r="79" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="15"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
-      <c r="I79" s="33"/>
-      <c r="J79" s="33"/>
-      <c r="K79" s="33"/>
-      <c r="L79" s="33"/>
-      <c r="M79" s="33"/>
-      <c r="N79" s="33"/>
-      <c r="O79" s="33"/>
-      <c r="P79" s="33"/>
-      <c r="Q79" s="33"/>
-      <c r="R79" s="33"/>
-      <c r="S79" s="33"/>
-      <c r="T79" s="33"/>
-      <c r="U79" s="33"/>
-      <c r="V79" s="33"/>
-      <c r="W79" s="33"/>
-      <c r="X79" s="33"/>
-      <c r="Y79" s="33"/>
-      <c r="Z79" s="33"/>
-      <c r="AA79" s="33"/>
-      <c r="AB79" s="33"/>
-      <c r="AC79" s="33"/>
-      <c r="AD79" s="33"/>
-      <c r="AE79" s="33"/>
-      <c r="AF79" s="33"/>
-      <c r="AG79" s="33"/>
-      <c r="AH79" s="33"/>
-      <c r="AI79" s="33"/>
-      <c r="AJ79" s="33"/>
-      <c r="AK79" s="33"/>
-      <c r="AL79" s="33"/>
-      <c r="AM79" s="33"/>
-      <c r="AN79" s="33"/>
-      <c r="AO79" s="33"/>
-      <c r="AP79" s="33"/>
-      <c r="AQ79" s="33"/>
-      <c r="AR79" s="34"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="36"/>
+      <c r="I79" s="36"/>
+      <c r="J79" s="36"/>
+      <c r="K79" s="36"/>
+      <c r="L79" s="36"/>
+      <c r="M79" s="36"/>
+      <c r="N79" s="36"/>
+      <c r="O79" s="36"/>
+      <c r="P79" s="36"/>
+      <c r="Q79" s="36"/>
+      <c r="R79" s="36"/>
+      <c r="S79" s="36"/>
+      <c r="T79" s="36"/>
+      <c r="U79" s="36"/>
+      <c r="V79" s="36"/>
+      <c r="W79" s="36"/>
+      <c r="X79" s="36"/>
+      <c r="Y79" s="36"/>
+      <c r="Z79" s="36"/>
+      <c r="AA79" s="36"/>
+      <c r="AB79" s="36"/>
+      <c r="AC79" s="36"/>
+      <c r="AD79" s="36"/>
+      <c r="AE79" s="36"/>
+      <c r="AF79" s="36"/>
+      <c r="AG79" s="36"/>
+      <c r="AH79" s="36"/>
+      <c r="AI79" s="36"/>
+      <c r="AJ79" s="36"/>
+      <c r="AK79" s="36"/>
+      <c r="AL79" s="36"/>
+      <c r="AM79" s="36"/>
+      <c r="AN79" s="36"/>
+      <c r="AO79" s="36"/>
+      <c r="AP79" s="36"/>
+      <c r="AQ79" s="36"/>
+      <c r="AR79" s="37"/>
     </row>
     <row r="80" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="15"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
-      <c r="H80" s="33"/>
-      <c r="I80" s="33"/>
-      <c r="J80" s="33"/>
-      <c r="K80" s="33"/>
-      <c r="L80" s="33"/>
-      <c r="M80" s="33"/>
-      <c r="N80" s="33"/>
-      <c r="O80" s="33"/>
-      <c r="P80" s="33"/>
-      <c r="Q80" s="33"/>
-      <c r="R80" s="33"/>
-      <c r="S80" s="33"/>
-      <c r="T80" s="33"/>
-      <c r="U80" s="33"/>
-      <c r="V80" s="33"/>
-      <c r="W80" s="33"/>
-      <c r="X80" s="33"/>
-      <c r="Y80" s="33"/>
-      <c r="Z80" s="33"/>
-      <c r="AA80" s="33"/>
-      <c r="AB80" s="33"/>
-      <c r="AC80" s="33"/>
-      <c r="AD80" s="33"/>
-      <c r="AE80" s="33"/>
-      <c r="AF80" s="33"/>
-      <c r="AG80" s="33"/>
-      <c r="AH80" s="33"/>
-      <c r="AI80" s="33"/>
-      <c r="AJ80" s="33"/>
-      <c r="AK80" s="33"/>
-      <c r="AL80" s="33"/>
-      <c r="AM80" s="33"/>
-      <c r="AN80" s="33"/>
-      <c r="AO80" s="33"/>
-      <c r="AP80" s="33"/>
-      <c r="AQ80" s="33"/>
-      <c r="AR80" s="34"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="36"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="36"/>
+      <c r="I80" s="36"/>
+      <c r="J80" s="36"/>
+      <c r="K80" s="36"/>
+      <c r="L80" s="36"/>
+      <c r="M80" s="36"/>
+      <c r="N80" s="36"/>
+      <c r="O80" s="36"/>
+      <c r="P80" s="36"/>
+      <c r="Q80" s="36"/>
+      <c r="R80" s="36"/>
+      <c r="S80" s="36"/>
+      <c r="T80" s="36"/>
+      <c r="U80" s="36"/>
+      <c r="V80" s="36"/>
+      <c r="W80" s="36"/>
+      <c r="X80" s="36"/>
+      <c r="Y80" s="36"/>
+      <c r="Z80" s="36"/>
+      <c r="AA80" s="36"/>
+      <c r="AB80" s="36"/>
+      <c r="AC80" s="36"/>
+      <c r="AD80" s="36"/>
+      <c r="AE80" s="36"/>
+      <c r="AF80" s="36"/>
+      <c r="AG80" s="36"/>
+      <c r="AH80" s="36"/>
+      <c r="AI80" s="36"/>
+      <c r="AJ80" s="36"/>
+      <c r="AK80" s="36"/>
+      <c r="AL80" s="36"/>
+      <c r="AM80" s="36"/>
+      <c r="AN80" s="36"/>
+      <c r="AO80" s="36"/>
+      <c r="AP80" s="36"/>
+      <c r="AQ80" s="36"/>
+      <c r="AR80" s="37"/>
     </row>
     <row r="81" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="15"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
-      <c r="H81" s="33"/>
-      <c r="I81" s="33"/>
-      <c r="J81" s="33"/>
-      <c r="K81" s="33"/>
-      <c r="L81" s="33"/>
-      <c r="M81" s="33"/>
-      <c r="N81" s="33"/>
-      <c r="O81" s="33"/>
-      <c r="P81" s="33"/>
-      <c r="Q81" s="33"/>
-      <c r="R81" s="33"/>
-      <c r="S81" s="33"/>
-      <c r="T81" s="33"/>
-      <c r="U81" s="33"/>
-      <c r="V81" s="33"/>
-      <c r="W81" s="33"/>
-      <c r="X81" s="33"/>
-      <c r="Y81" s="33"/>
-      <c r="Z81" s="33"/>
-      <c r="AA81" s="33"/>
-      <c r="AB81" s="33"/>
-      <c r="AC81" s="33"/>
-      <c r="AD81" s="33"/>
-      <c r="AE81" s="33"/>
-      <c r="AF81" s="33"/>
-      <c r="AG81" s="33"/>
-      <c r="AH81" s="33"/>
-      <c r="AI81" s="33"/>
-      <c r="AJ81" s="33"/>
-      <c r="AK81" s="33"/>
-      <c r="AL81" s="33"/>
-      <c r="AM81" s="33"/>
-      <c r="AN81" s="33"/>
-      <c r="AO81" s="33"/>
-      <c r="AP81" s="33"/>
-      <c r="AQ81" s="33"/>
-      <c r="AR81" s="34"/>
-    </row>
-    <row r="82" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="36"/>
+      <c r="I81" s="36"/>
+      <c r="J81" s="36"/>
+      <c r="K81" s="36"/>
+      <c r="L81" s="36"/>
+      <c r="M81" s="36"/>
+      <c r="N81" s="36"/>
+      <c r="O81" s="36"/>
+      <c r="P81" s="36"/>
+      <c r="Q81" s="36"/>
+      <c r="R81" s="36"/>
+      <c r="S81" s="36"/>
+      <c r="T81" s="36"/>
+      <c r="U81" s="36"/>
+      <c r="V81" s="36"/>
+      <c r="W81" s="36"/>
+      <c r="X81" s="36"/>
+      <c r="Y81" s="36"/>
+      <c r="Z81" s="36"/>
+      <c r="AA81" s="36"/>
+      <c r="AB81" s="36"/>
+      <c r="AC81" s="36"/>
+      <c r="AD81" s="36"/>
+      <c r="AE81" s="36"/>
+      <c r="AF81" s="36"/>
+      <c r="AG81" s="36"/>
+      <c r="AH81" s="36"/>
+      <c r="AI81" s="36"/>
+      <c r="AJ81" s="36"/>
+      <c r="AK81" s="36"/>
+      <c r="AL81" s="36"/>
+      <c r="AM81" s="36"/>
+      <c r="AN81" s="36"/>
+      <c r="AO81" s="36"/>
+      <c r="AP81" s="36"/>
+      <c r="AQ81" s="36"/>
+      <c r="AR81" s="37"/>
+    </row>
+    <row r="82" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="15"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
-      <c r="H82" s="33"/>
-      <c r="I82" s="33"/>
-      <c r="J82" s="33"/>
-      <c r="K82" s="33"/>
-      <c r="L82" s="33"/>
-      <c r="M82" s="33"/>
-      <c r="N82" s="33"/>
-      <c r="O82" s="33"/>
-      <c r="P82" s="33"/>
-      <c r="Q82" s="33"/>
-      <c r="R82" s="33"/>
-      <c r="S82" s="33"/>
-      <c r="T82" s="33"/>
-      <c r="U82" s="33"/>
-      <c r="V82" s="33"/>
-      <c r="W82" s="33"/>
-      <c r="X82" s="33"/>
-      <c r="Y82" s="33"/>
-      <c r="Z82" s="33"/>
-      <c r="AA82" s="33"/>
-      <c r="AB82" s="33"/>
-      <c r="AC82" s="33"/>
-      <c r="AD82" s="33"/>
-      <c r="AE82" s="33"/>
-      <c r="AF82" s="33"/>
-      <c r="AG82" s="33"/>
-      <c r="AH82" s="33"/>
-      <c r="AI82" s="33"/>
-      <c r="AJ82" s="33"/>
-      <c r="AK82" s="33"/>
-      <c r="AL82" s="33"/>
-      <c r="AM82" s="33"/>
-      <c r="AN82" s="33"/>
-      <c r="AO82" s="33"/>
-      <c r="AP82" s="33"/>
-      <c r="AQ82" s="33"/>
-      <c r="AR82" s="34"/>
-    </row>
-    <row r="83" spans="2:44" ht="15" x14ac:dyDescent="0.25">
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="36"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="36"/>
+      <c r="N82" s="36"/>
+      <c r="O82" s="36"/>
+      <c r="P82" s="36"/>
+      <c r="Q82" s="36"/>
+      <c r="R82" s="36"/>
+      <c r="S82" s="36"/>
+      <c r="T82" s="36"/>
+      <c r="U82" s="36"/>
+      <c r="V82" s="36"/>
+      <c r="W82" s="36"/>
+      <c r="X82" s="36"/>
+      <c r="Y82" s="36"/>
+      <c r="Z82" s="36"/>
+      <c r="AA82" s="36"/>
+      <c r="AB82" s="36"/>
+      <c r="AC82" s="36"/>
+      <c r="AD82" s="36"/>
+      <c r="AE82" s="36"/>
+      <c r="AF82" s="36"/>
+      <c r="AG82" s="36"/>
+      <c r="AH82" s="36"/>
+      <c r="AI82" s="36"/>
+      <c r="AJ82" s="36"/>
+      <c r="AK82" s="36"/>
+      <c r="AL82" s="36"/>
+      <c r="AM82" s="36"/>
+      <c r="AN82" s="36"/>
+      <c r="AO82" s="36"/>
+      <c r="AP82" s="36"/>
+      <c r="AQ82" s="36"/>
+      <c r="AR82" s="37"/>
+    </row>
+    <row r="83" spans="2:44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="15"/>
-      <c r="AC83" s="8"/>
-      <c r="AR83" s="16"/>
-    </row>
-    <row r="84" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="C83" s="36"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="36"/>
+      <c r="I83" s="36"/>
+      <c r="J83" s="36"/>
+      <c r="K83" s="36"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="36"/>
+      <c r="N83" s="36"/>
+      <c r="O83" s="36"/>
+      <c r="P83" s="36"/>
+      <c r="Q83" s="36"/>
+      <c r="R83" s="36"/>
+      <c r="S83" s="36"/>
+      <c r="T83" s="36"/>
+      <c r="U83" s="36"/>
+      <c r="V83" s="36"/>
+      <c r="W83" s="36"/>
+      <c r="X83" s="36"/>
+      <c r="Y83" s="36"/>
+      <c r="Z83" s="36"/>
+      <c r="AA83" s="36"/>
+      <c r="AB83" s="36"/>
+      <c r="AC83" s="36"/>
+      <c r="AD83" s="36"/>
+      <c r="AE83" s="36"/>
+      <c r="AF83" s="36"/>
+      <c r="AG83" s="36"/>
+      <c r="AH83" s="36"/>
+      <c r="AI83" s="36"/>
+      <c r="AJ83" s="36"/>
+      <c r="AK83" s="36"/>
+      <c r="AL83" s="36"/>
+      <c r="AM83" s="36"/>
+      <c r="AN83" s="36"/>
+      <c r="AO83" s="36"/>
+      <c r="AP83" s="36"/>
+      <c r="AQ83" s="36"/>
+      <c r="AR83" s="37"/>
+    </row>
+    <row r="84" spans="2:44" ht="15" x14ac:dyDescent="0.25">
       <c r="B84" s="15"/>
+      <c r="AC84" s="8"/>
       <c r="AR84" s="16"/>
     </row>
     <row r="85" spans="2:44" x14ac:dyDescent="0.2">
@@ -6423,56 +6490,59 @@
       <c r="B95" s="15"/>
       <c r="AR95" s="16"/>
     </row>
-    <row r="96" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="18"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="19"/>
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
-      <c r="J96" s="19"/>
-      <c r="K96" s="19"/>
-      <c r="L96" s="19"/>
-      <c r="M96" s="19"/>
-      <c r="N96" s="19"/>
-      <c r="O96" s="19"/>
-      <c r="P96" s="19"/>
-      <c r="Q96" s="19"/>
-      <c r="R96" s="19"/>
-      <c r="S96" s="19"/>
-      <c r="T96" s="19"/>
-      <c r="U96" s="19"/>
-      <c r="V96" s="19"/>
-      <c r="W96" s="19"/>
-      <c r="X96" s="19"/>
-      <c r="Y96" s="19"/>
-      <c r="Z96" s="19"/>
-      <c r="AA96" s="19"/>
-      <c r="AB96" s="19"/>
-      <c r="AC96" s="19"/>
-      <c r="AD96" s="19"/>
-      <c r="AE96" s="19"/>
-      <c r="AF96" s="19"/>
-      <c r="AG96" s="19"/>
-      <c r="AH96" s="19"/>
-      <c r="AI96" s="19"/>
-      <c r="AJ96" s="19"/>
-      <c r="AK96" s="19"/>
-      <c r="AL96" s="19"/>
-      <c r="AM96" s="19"/>
-      <c r="AN96" s="19"/>
-      <c r="AO96" s="19"/>
-      <c r="AP96" s="19"/>
-      <c r="AQ96" s="19"/>
-      <c r="AR96" s="20"/>
+    <row r="96" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="B96" s="15"/>
+      <c r="AR96" s="16"/>
+    </row>
+    <row r="97" spans="2:44" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="18"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
+      <c r="J97" s="19"/>
+      <c r="K97" s="19"/>
+      <c r="L97" s="19"/>
+      <c r="M97" s="19"/>
+      <c r="N97" s="19"/>
+      <c r="O97" s="19"/>
+      <c r="P97" s="19"/>
+      <c r="Q97" s="19"/>
+      <c r="R97" s="19"/>
+      <c r="S97" s="19"/>
+      <c r="T97" s="19"/>
+      <c r="U97" s="19"/>
+      <c r="V97" s="19"/>
+      <c r="W97" s="19"/>
+      <c r="X97" s="19"/>
+      <c r="Y97" s="19"/>
+      <c r="Z97" s="19"/>
+      <c r="AA97" s="19"/>
+      <c r="AB97" s="19"/>
+      <c r="AC97" s="19"/>
+      <c r="AD97" s="19"/>
+      <c r="AE97" s="19"/>
+      <c r="AF97" s="19"/>
+      <c r="AG97" s="19"/>
+      <c r="AH97" s="19"/>
+      <c r="AI97" s="19"/>
+      <c r="AJ97" s="19"/>
+      <c r="AK97" s="19"/>
+      <c r="AL97" s="19"/>
+      <c r="AM97" s="19"/>
+      <c r="AN97" s="19"/>
+      <c r="AO97" s="19"/>
+      <c r="AP97" s="19"/>
+      <c r="AQ97" s="19"/>
+      <c r="AR97" s="20"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="10">
-    <mergeCell ref="C82:AR82"/>
-    <mergeCell ref="C73:AR73"/>
+    <mergeCell ref="C83:AR83"/>
     <mergeCell ref="C74:AR74"/>
     <mergeCell ref="C75:AR75"/>
     <mergeCell ref="C76:AR76"/>
@@ -6481,6 +6551,7 @@
     <mergeCell ref="C79:AR79"/>
     <mergeCell ref="C80:AR80"/>
     <mergeCell ref="C81:AR81"/>
+    <mergeCell ref="C82:AR82"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{8700012B-1663-4F72-A9B4-B92390B41D1E}"/>
@@ -6745,9 +6816,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6895,26 +6969,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6938,9 +7001,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>